<commit_message>
Abschluss WSK + Auswertung OPS
</commit_message>
<xml_diff>
--- a/9 - WSK/Auswertung/Entladekurve.xlsx
+++ b/9 - WSK/Auswertung/Entladekurve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicoe\Files\Studium\Grundpraktikum\9 - WSK\Auswertung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sstah\Documents\GP2\Grundpraktikum-2-main\9 - WSK\Auswertung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66FEBBC-6010-4A76-B046-93E716E99E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61203586-07A5-486C-979A-3508AB6B1BC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>t in ms</t>
   </si>
   <si>
     <t>U in div</t>
-  </si>
-  <si>
-    <t>beides Mal Fehler 0,1</t>
   </si>
 </sst>
 </file>
@@ -362,15 +359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,7 +375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -386,7 +383,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.6</v>
       </c>
@@ -394,7 +391,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -402,7 +399,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.8</v>
       </c>
@@ -410,7 +407,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2.4</v>
       </c>
@@ -418,7 +415,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -426,7 +423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3.6</v>
       </c>
@@ -434,7 +431,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>4.2</v>
       </c>
@@ -442,7 +439,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>4.8</v>
       </c>
@@ -450,17 +447,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>5.4</v>
       </c>
       <c r="B11">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>